<commit_message>
Current Update: Most Recent File
</commit_message>
<xml_diff>
--- a/SessionBackup/LastSessionItems.xlsx
+++ b/SessionBackup/LastSessionItems.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SorazaImport\Desktop\barcodevba\SessionBackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF2C457-EA5C-4830-BF7D-86E4E69CEE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C349171-13CC-42E3-A329-D2981D1ADC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Productos!$B$3:$B$3961</definedName>
+  </definedNames>
   <calcPr calcId="191029" forceFullCalc="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7914" uniqueCount="4907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7926" uniqueCount="4913">
   <si>
     <t>#</t>
   </si>
@@ -14754,6 +14757,24 @@
   </si>
   <si>
     <t>Manicura</t>
+  </si>
+  <si>
+    <t>WB001</t>
+  </si>
+  <si>
+    <t>WQ001</t>
+  </si>
+  <si>
+    <t>WT001</t>
+  </si>
+  <si>
+    <t>WT002</t>
+  </si>
+  <si>
+    <t>WW001</t>
+  </si>
+  <si>
+    <t>WB002</t>
   </si>
 </sst>
 </file>
@@ -15094,10 +15115,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A3:L3954"/>
+  <dimension ref="A3:L3960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3902" workbookViewId="0">
-      <selection activeCell="B3936" sqref="B3936"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56733,65 +56754,65 @@
     </row>
     <row r="3785" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3785" t="s">
-        <v>4882</v>
+        <v>4907</v>
       </c>
       <c r="E3785" t="s">
-        <v>3161</v>
+        <v>86</v>
       </c>
       <c r="K3785">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3786" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3786" t="s">
-        <v>4883</v>
+        <v>4912</v>
       </c>
       <c r="E3786" t="s">
-        <v>3264</v>
+        <v>86</v>
       </c>
       <c r="K3786">
-        <v>25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3787" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3787" t="s">
-        <v>4884</v>
+        <v>4908</v>
       </c>
       <c r="E3787" t="s">
-        <v>4887</v>
+        <v>149</v>
       </c>
       <c r="K3787">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3788" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3788" t="s">
-        <v>2882</v>
+        <v>4909</v>
       </c>
       <c r="E3788" t="s">
-        <v>1021</v>
+        <v>3686</v>
       </c>
       <c r="K3788">
-        <v>2.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3789" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3789" t="s">
-        <v>4885</v>
+        <v>4910</v>
       </c>
       <c r="E3789" t="s">
-        <v>4888</v>
+        <v>4862</v>
       </c>
       <c r="K3789">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3790" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3790" t="s">
-        <v>4886</v>
+        <v>4911</v>
       </c>
       <c r="E3790" t="s">
-        <v>4893</v>
+        <v>365</v>
       </c>
       <c r="K3790">
         <v>15</v>
@@ -56799,32 +56820,32 @@
     </row>
     <row r="3791" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3791" t="s">
-        <v>991</v>
+        <v>4882</v>
       </c>
       <c r="E3791" t="s">
-        <v>992</v>
+        <v>3161</v>
       </c>
       <c r="K3791">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3792" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3792" t="s">
-        <v>984</v>
+        <v>4883</v>
       </c>
       <c r="E3792" t="s">
-        <v>985</v>
+        <v>3264</v>
       </c>
       <c r="K3792">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3793" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3793" t="s">
-        <v>2812</v>
+        <v>4884</v>
       </c>
       <c r="E3793" t="s">
-        <v>2797</v>
+        <v>4887</v>
       </c>
       <c r="K3793">
         <v>15</v>
@@ -56832,131 +56853,131 @@
     </row>
     <row r="3794" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3794" t="s">
-        <v>2868</v>
+        <v>2882</v>
       </c>
       <c r="E3794" t="s">
-        <v>1016</v>
+        <v>1021</v>
       </c>
       <c r="K3794">
-        <v>12</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3795" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3795" t="s">
-        <v>2809</v>
+        <v>4885</v>
       </c>
       <c r="E3795" t="s">
-        <v>2797</v>
+        <v>4888</v>
       </c>
       <c r="K3795">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3796" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3796" t="s">
-        <v>2790</v>
+        <v>4886</v>
       </c>
       <c r="E3796" t="s">
-        <v>573</v>
+        <v>4893</v>
       </c>
       <c r="K3796">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3797" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3797" t="s">
-        <v>2705</v>
+        <v>991</v>
       </c>
       <c r="E3797" t="s">
-        <v>999</v>
+        <v>992</v>
       </c>
       <c r="K3797">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3798" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3798" t="s">
-        <v>2808</v>
+        <v>984</v>
       </c>
       <c r="E3798" t="s">
-        <v>2797</v>
+        <v>985</v>
       </c>
       <c r="K3798">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3799" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3799" t="s">
-        <v>986</v>
+        <v>2812</v>
       </c>
       <c r="E3799" t="s">
-        <v>985</v>
+        <v>2797</v>
       </c>
       <c r="K3799">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3800" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3800" t="s">
-        <v>1009</v>
+        <v>2868</v>
       </c>
       <c r="E3800" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="K3800">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3801" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3801" t="s">
-        <v>995</v>
+        <v>2809</v>
       </c>
       <c r="E3801" t="s">
-        <v>996</v>
+        <v>2797</v>
       </c>
       <c r="K3801">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3802" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3802" t="s">
-        <v>1003</v>
+        <v>2790</v>
       </c>
       <c r="E3802" t="s">
-        <v>1004</v>
+        <v>573</v>
       </c>
       <c r="K3802">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3803" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3803" t="s">
-        <v>1005</v>
+        <v>2705</v>
       </c>
       <c r="E3803" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
       <c r="K3803">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3804" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3804" t="s">
-        <v>1007</v>
+        <v>2808</v>
       </c>
       <c r="E3804" t="s">
-        <v>1008</v>
+        <v>2797</v>
       </c>
       <c r="K3804">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3805" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3805" t="s">
-        <v>1000</v>
+        <v>986</v>
       </c>
       <c r="E3805" t="s">
-        <v>1001</v>
+        <v>985</v>
       </c>
       <c r="K3805">
         <v>18</v>
@@ -56964,131 +56985,131 @@
     </row>
     <row r="3806" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3806" t="s">
-        <v>1002</v>
+        <v>1009</v>
       </c>
       <c r="E3806" t="s">
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="K3806">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3807" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3807" t="s">
-        <v>987</v>
+        <v>995</v>
       </c>
       <c r="E3807" t="s">
-        <v>985</v>
+        <v>996</v>
       </c>
       <c r="K3807">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3808" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3808" t="s">
-        <v>1011</v>
+        <v>1003</v>
       </c>
       <c r="E3808" t="s">
-        <v>1012</v>
+        <v>1004</v>
       </c>
       <c r="K3808">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3809" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3809" t="s">
-        <v>1023</v>
+        <v>1005</v>
       </c>
       <c r="E3809" t="s">
-        <v>1024</v>
+        <v>1004</v>
       </c>
       <c r="K3809">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3810" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3810" t="s">
-        <v>997</v>
+        <v>1007</v>
       </c>
       <c r="E3810" t="s">
-        <v>996</v>
+        <v>1008</v>
       </c>
       <c r="K3810">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3811" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3811" t="s">
-        <v>993</v>
+        <v>1000</v>
       </c>
       <c r="E3811" t="s">
-        <v>992</v>
+        <v>1001</v>
       </c>
       <c r="K3811">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3812" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3812" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
       <c r="E3812" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="K3812">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3813" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3813" t="s">
-        <v>994</v>
+        <v>987</v>
       </c>
       <c r="E3813" t="s">
-        <v>992</v>
+        <v>985</v>
       </c>
       <c r="K3813">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3814" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3814" t="s">
-        <v>988</v>
+        <v>1011</v>
       </c>
       <c r="E3814" t="s">
-        <v>985</v>
+        <v>1012</v>
       </c>
       <c r="K3814">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3815" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3815" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="E3815" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K3815">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3816" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3816" t="s">
-        <v>1027</v>
+        <v>997</v>
       </c>
       <c r="E3816" t="s">
-        <v>1026</v>
+        <v>996</v>
       </c>
       <c r="K3816">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3817" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3817" t="s">
-        <v>1017</v>
+        <v>993</v>
       </c>
       <c r="E3817" t="s">
-        <v>1018</v>
+        <v>992</v>
       </c>
       <c r="K3817">
         <v>16</v>
@@ -57096,238 +57117,238 @@
     </row>
     <row r="3818" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3818" t="s">
-        <v>1019</v>
+        <v>1006</v>
       </c>
       <c r="E3818" t="s">
-        <v>1018</v>
+        <v>1004</v>
       </c>
       <c r="K3818">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3819" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3819" t="s">
-        <v>1028</v>
+        <v>994</v>
       </c>
       <c r="E3819" t="s">
-        <v>1026</v>
+        <v>992</v>
       </c>
       <c r="K3819">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3820" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3820" t="s">
-        <v>1020</v>
+        <v>988</v>
       </c>
       <c r="E3820" t="s">
-        <v>1021</v>
+        <v>985</v>
       </c>
       <c r="K3820">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3821" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3821" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="E3821" t="s">
-        <v>1021</v>
+        <v>1026</v>
       </c>
       <c r="K3821">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3822" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3822" t="s">
-        <v>1015</v>
+        <v>1027</v>
       </c>
       <c r="E3822" t="s">
-        <v>1016</v>
+        <v>1026</v>
       </c>
       <c r="K3822">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3823" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3823" t="s">
-        <v>989</v>
+        <v>1017</v>
       </c>
       <c r="E3823" t="s">
-        <v>990</v>
+        <v>1018</v>
       </c>
       <c r="K3823">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3824" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3824" t="s">
-        <v>1013</v>
+        <v>1019</v>
       </c>
       <c r="E3824" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="K3824">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3825" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3825" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="E3825" t="s">
         <v>1026</v>
       </c>
       <c r="K3825">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3826" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3826" t="s">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="E3826" t="s">
-        <v>1026</v>
+        <v>1021</v>
       </c>
       <c r="K3826">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3827" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3827" t="s">
-        <v>998</v>
+        <v>1022</v>
       </c>
       <c r="E3827" t="s">
-        <v>999</v>
+        <v>1021</v>
       </c>
       <c r="K3827">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3828" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3828" t="s">
-        <v>2691</v>
+        <v>1015</v>
       </c>
       <c r="E3828" t="s">
-        <v>992</v>
+        <v>1016</v>
       </c>
       <c r="K3828">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3829" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3829" t="s">
-        <v>2811</v>
+        <v>989</v>
       </c>
       <c r="E3829" t="s">
-        <v>2797</v>
+        <v>990</v>
       </c>
       <c r="K3829">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3830" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3830" t="s">
-        <v>2694</v>
+        <v>1013</v>
       </c>
       <c r="E3830" t="s">
-        <v>992</v>
+        <v>1014</v>
       </c>
       <c r="K3830">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3831" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3831" t="s">
-        <v>2692</v>
+        <v>1029</v>
       </c>
       <c r="E3831" t="s">
-        <v>992</v>
+        <v>1026</v>
       </c>
       <c r="K3831">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3832" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3832" t="s">
-        <v>2805</v>
+        <v>1030</v>
       </c>
       <c r="E3832" t="s">
-        <v>2797</v>
+        <v>1026</v>
       </c>
       <c r="K3832">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3833" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3833" t="s">
-        <v>2867</v>
+        <v>998</v>
       </c>
       <c r="E3833" t="s">
-        <v>2687</v>
+        <v>999</v>
       </c>
       <c r="K3833">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3834" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3834" t="s">
-        <v>2865</v>
+        <v>2691</v>
       </c>
       <c r="E3834" t="s">
-        <v>2866</v>
+        <v>992</v>
       </c>
       <c r="K3834">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3835" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3835" t="s">
-        <v>2649</v>
+        <v>2811</v>
       </c>
       <c r="E3835" t="s">
-        <v>985</v>
+        <v>2797</v>
       </c>
       <c r="K3835">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3836" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3836" t="s">
-        <v>2650</v>
+        <v>2694</v>
       </c>
       <c r="E3836" t="s">
-        <v>985</v>
+        <v>992</v>
       </c>
       <c r="K3836">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3837" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3837" t="s">
-        <v>2810</v>
+        <v>2692</v>
       </c>
       <c r="E3837" t="s">
-        <v>2797</v>
+        <v>992</v>
       </c>
       <c r="K3837">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3838" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3838" t="s">
-        <v>2881</v>
+        <v>2805</v>
       </c>
       <c r="E3838" t="s">
-        <v>1021</v>
+        <v>2797</v>
       </c>
       <c r="K3838">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3839" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3839" t="s">
-        <v>2887</v>
+        <v>2867</v>
       </c>
       <c r="E3839" t="s">
         <v>2687</v>
@@ -57338,98 +57359,98 @@
     </row>
     <row r="3840" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3840" t="s">
-        <v>2870</v>
+        <v>2865</v>
       </c>
       <c r="E3840" t="s">
-        <v>1016</v>
+        <v>2866</v>
       </c>
       <c r="K3840">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3841" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3841" t="s">
-        <v>2779</v>
+        <v>2649</v>
       </c>
       <c r="E3841" t="s">
-        <v>2289</v>
+        <v>985</v>
       </c>
       <c r="K3841">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3842" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3842" t="s">
-        <v>2782</v>
+        <v>2650</v>
       </c>
       <c r="E3842" t="s">
-        <v>2783</v>
+        <v>985</v>
       </c>
       <c r="K3842">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3843" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3843" t="s">
-        <v>2883</v>
+        <v>2810</v>
       </c>
       <c r="E3843" t="s">
-        <v>1021</v>
+        <v>2797</v>
       </c>
       <c r="K3843">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3844" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3844" t="s">
-        <v>2718</v>
+        <v>2881</v>
       </c>
       <c r="E3844" t="s">
-        <v>2715</v>
+        <v>1021</v>
       </c>
       <c r="K3844">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3845" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3845" t="s">
-        <v>2689</v>
+        <v>2887</v>
       </c>
       <c r="E3845" t="s">
-        <v>2690</v>
+        <v>2687</v>
       </c>
       <c r="K3845">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3846" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3846" t="s">
-        <v>2658</v>
+        <v>2870</v>
       </c>
       <c r="E3846" t="s">
-        <v>2659</v>
+        <v>1016</v>
       </c>
       <c r="K3846">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3847" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3847" t="s">
-        <v>2660</v>
+        <v>2779</v>
       </c>
       <c r="E3847" t="s">
-        <v>2659</v>
+        <v>2289</v>
       </c>
       <c r="K3847">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3848" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3848" t="s">
-        <v>2665</v>
+        <v>2782</v>
       </c>
       <c r="E3848" t="s">
-        <v>2666</v>
+        <v>2783</v>
       </c>
       <c r="K3848">
         <v>5</v>
@@ -57437,197 +57458,197 @@
     </row>
     <row r="3849" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3849" t="s">
-        <v>2813</v>
+        <v>2883</v>
       </c>
       <c r="E3849" t="s">
-        <v>2814</v>
+        <v>1021</v>
       </c>
       <c r="K3849">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3850" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3850" t="s">
-        <v>2792</v>
+        <v>2718</v>
       </c>
       <c r="E3850" t="s">
-        <v>2793</v>
+        <v>2715</v>
       </c>
       <c r="K3850">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3851" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3851" t="s">
-        <v>2686</v>
+        <v>2689</v>
       </c>
       <c r="E3851" t="s">
-        <v>2687</v>
+        <v>2690</v>
       </c>
       <c r="K3851">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3852" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3852" t="s">
-        <v>2688</v>
+        <v>2658</v>
       </c>
       <c r="E3852" t="s">
-        <v>2687</v>
+        <v>2659</v>
       </c>
       <c r="K3852">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3853" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3853" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="E3853" t="s">
         <v>2659</v>
       </c>
       <c r="K3853">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3854" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3854" t="s">
-        <v>2806</v>
+        <v>2665</v>
       </c>
       <c r="E3854" t="s">
-        <v>2797</v>
+        <v>2666</v>
       </c>
       <c r="K3854">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3855" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3855" t="s">
-        <v>2807</v>
+        <v>2813</v>
       </c>
       <c r="E3855" t="s">
-        <v>2797</v>
+        <v>2814</v>
       </c>
       <c r="K3855">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3856" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3856" t="s">
-        <v>2693</v>
+        <v>2792</v>
       </c>
       <c r="E3856" t="s">
-        <v>992</v>
+        <v>2793</v>
       </c>
       <c r="K3856">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3857" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3857" t="s">
-        <v>2662</v>
+        <v>2686</v>
       </c>
       <c r="E3857" t="s">
-        <v>2659</v>
+        <v>2687</v>
       </c>
       <c r="K3857">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3858" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3858" t="s">
-        <v>2869</v>
+        <v>2688</v>
       </c>
       <c r="E3858" t="s">
-        <v>1016</v>
+        <v>2687</v>
       </c>
       <c r="K3858">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3859" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3859" t="s">
-        <v>2875</v>
+        <v>2661</v>
       </c>
       <c r="E3859" t="s">
-        <v>2876</v>
+        <v>2659</v>
       </c>
       <c r="K3859">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3860" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3860" t="s">
-        <v>2679</v>
+        <v>2806</v>
       </c>
       <c r="E3860" t="s">
-        <v>2680</v>
+        <v>2797</v>
       </c>
       <c r="K3860">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3861" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3861" t="s">
-        <v>2731</v>
+        <v>2807</v>
       </c>
       <c r="E3861" t="s">
-        <v>2732</v>
+        <v>2797</v>
       </c>
       <c r="K3861">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3862" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3862" t="s">
-        <v>3252</v>
+        <v>2693</v>
       </c>
       <c r="E3862" t="s">
-        <v>1016</v>
+        <v>992</v>
       </c>
       <c r="K3862">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3863" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3863" t="s">
-        <v>3253</v>
+        <v>2662</v>
       </c>
       <c r="E3863" t="s">
-        <v>3254</v>
+        <v>2659</v>
       </c>
       <c r="K3863">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3864" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3864" t="s">
-        <v>3255</v>
+        <v>2869</v>
       </c>
       <c r="E3864" t="s">
-        <v>3254</v>
+        <v>1016</v>
       </c>
       <c r="K3864">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3865" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3865" t="s">
-        <v>3256</v>
+        <v>2875</v>
       </c>
       <c r="E3865" t="s">
-        <v>2687</v>
+        <v>2876</v>
       </c>
       <c r="K3865">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3866" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3866" t="s">
-        <v>3257</v>
+        <v>2679</v>
       </c>
       <c r="E3866" t="s">
-        <v>3258</v>
+        <v>2680</v>
       </c>
       <c r="K3866">
         <v>12</v>
@@ -57635,98 +57656,98 @@
     </row>
     <row r="3867" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3867" t="s">
-        <v>3260</v>
+        <v>2731</v>
       </c>
       <c r="E3867" t="s">
-        <v>2797</v>
+        <v>2732</v>
       </c>
       <c r="K3867">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3868" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3868" t="s">
-        <v>3261</v>
+        <v>3252</v>
       </c>
       <c r="E3868" t="s">
-        <v>3262</v>
+        <v>1016</v>
       </c>
       <c r="K3868">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3869" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3869" t="s">
-        <v>3160</v>
+        <v>3253</v>
       </c>
       <c r="E3869" t="s">
-        <v>3161</v>
+        <v>3254</v>
       </c>
       <c r="K3869">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3870" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3870" t="s">
-        <v>3263</v>
+        <v>3255</v>
       </c>
       <c r="E3870" t="s">
-        <v>3264</v>
+        <v>3254</v>
       </c>
       <c r="K3870">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3871" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3871" t="s">
-        <v>3546</v>
+        <v>3256</v>
       </c>
       <c r="E3871" t="s">
-        <v>2481</v>
+        <v>2687</v>
       </c>
       <c r="K3871">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3872" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3872" t="s">
-        <v>3547</v>
+        <v>3257</v>
       </c>
       <c r="E3872" t="s">
-        <v>2700</v>
+        <v>3258</v>
       </c>
       <c r="K3872">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3873" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3873" t="s">
-        <v>3548</v>
+        <v>3260</v>
       </c>
       <c r="E3873" t="s">
         <v>2797</v>
       </c>
       <c r="K3873">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3874" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3874" t="s">
-        <v>3549</v>
+        <v>3261</v>
       </c>
       <c r="E3874" t="s">
-        <v>2797</v>
+        <v>3262</v>
       </c>
       <c r="K3874">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3875" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3875" t="s">
-        <v>3550</v>
+        <v>3160</v>
       </c>
       <c r="E3875" t="s">
-        <v>3551</v>
+        <v>3161</v>
       </c>
       <c r="K3875">
         <v>22</v>
@@ -57734,384 +57755,384 @@
     </row>
     <row r="3876" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3876" t="s">
-        <v>3552</v>
+        <v>3263</v>
       </c>
       <c r="E3876" t="s">
-        <v>3553</v>
+        <v>3264</v>
       </c>
       <c r="K3876">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3877" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3877" t="s">
-        <v>3554</v>
+        <v>3546</v>
       </c>
       <c r="E3877" t="s">
-        <v>3555</v>
+        <v>2481</v>
       </c>
       <c r="K3877">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3878" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3878" t="s">
-        <v>4123</v>
+        <v>3547</v>
       </c>
       <c r="E3878" t="s">
-        <v>1016</v>
+        <v>2700</v>
       </c>
       <c r="K3878">
-        <v>285</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3879" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3879" t="s">
-        <v>4124</v>
+        <v>3548</v>
       </c>
       <c r="E3879" t="s">
-        <v>3469</v>
+        <v>2797</v>
       </c>
       <c r="K3879">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3880" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3880" t="s">
-        <v>4308</v>
+        <v>3549</v>
       </c>
       <c r="E3880" t="s">
-        <v>4309</v>
+        <v>2797</v>
       </c>
       <c r="K3880">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3881" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3881" t="s">
-        <v>4310</v>
+        <v>3550</v>
       </c>
       <c r="E3881" t="s">
-        <v>2680</v>
+        <v>3551</v>
       </c>
       <c r="K3881">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3882" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3882" t="s">
-        <v>4384</v>
+        <v>3552</v>
       </c>
       <c r="E3882" t="s">
-        <v>1014</v>
+        <v>3553</v>
       </c>
       <c r="K3882">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3883" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3883" t="s">
-        <v>4416</v>
+        <v>3554</v>
       </c>
       <c r="E3883" t="s">
-        <v>1570</v>
+        <v>3555</v>
       </c>
       <c r="K3883">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3884" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3884" t="s">
-        <v>4417</v>
+        <v>4123</v>
       </c>
       <c r="E3884" t="s">
-        <v>1077</v>
+        <v>1016</v>
       </c>
       <c r="K3884">
-        <v>10</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3885" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3885" t="s">
-        <v>4512</v>
+        <v>4124</v>
       </c>
       <c r="E3885" t="s">
-        <v>573</v>
+        <v>3469</v>
       </c>
       <c r="K3885">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3886" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3886" t="s">
-        <v>4513</v>
+        <v>4308</v>
       </c>
       <c r="E3886" t="s">
-        <v>2141</v>
+        <v>4309</v>
       </c>
       <c r="K3886">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3887" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3887" t="s">
-        <v>4543</v>
+        <v>4310</v>
       </c>
       <c r="E3887" t="s">
-        <v>990</v>
+        <v>2680</v>
       </c>
       <c r="K3887">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3888" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3888" t="s">
-        <v>4657</v>
+        <v>4384</v>
       </c>
       <c r="E3888" t="s">
-        <v>2481</v>
+        <v>1014</v>
       </c>
       <c r="K3888">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3889" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3889" t="s">
-        <v>4658</v>
+        <v>4416</v>
       </c>
       <c r="E3889" t="s">
-        <v>2481</v>
+        <v>1570</v>
       </c>
       <c r="K3889">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3890" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3890" t="s">
-        <v>4771</v>
+        <v>4417</v>
       </c>
       <c r="E3890" t="s">
-        <v>1570</v>
+        <v>1077</v>
       </c>
       <c r="K3890">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3891" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3891" t="s">
-        <v>4820</v>
+        <v>4512</v>
       </c>
       <c r="E3891" t="s">
-        <v>2715</v>
+        <v>573</v>
       </c>
       <c r="K3891">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3892" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3892" t="s">
-        <v>4821</v>
+        <v>4513</v>
       </c>
       <c r="E3892" t="s">
-        <v>2715</v>
+        <v>2141</v>
       </c>
       <c r="K3892">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3893" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3893" t="s">
-        <v>4822</v>
+        <v>4543</v>
       </c>
       <c r="E3893" t="s">
-        <v>2715</v>
+        <v>990</v>
       </c>
       <c r="K3893">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3894" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3894" t="s">
-        <v>1265</v>
+        <v>4657</v>
       </c>
       <c r="E3894" t="s">
-        <v>1266</v>
+        <v>2481</v>
       </c>
       <c r="K3894">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3895" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3895" t="s">
-        <v>1267</v>
+        <v>4658</v>
       </c>
       <c r="E3895" t="s">
-        <v>1266</v>
+        <v>2481</v>
       </c>
       <c r="K3895">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3896" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3896" t="s">
-        <v>1227</v>
+        <v>4771</v>
       </c>
       <c r="E3896" t="s">
-        <v>497</v>
+        <v>1570</v>
       </c>
       <c r="K3896">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3897" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3897" t="s">
-        <v>1228</v>
+        <v>4820</v>
       </c>
       <c r="E3897" t="s">
-        <v>497</v>
+        <v>2715</v>
       </c>
       <c r="K3897">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3898" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3898" t="s">
-        <v>1261</v>
+        <v>4821</v>
       </c>
       <c r="E3898" t="s">
-        <v>1262</v>
+        <v>2715</v>
       </c>
       <c r="K3898">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3899" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3899" t="s">
-        <v>1252</v>
+        <v>4822</v>
       </c>
       <c r="E3899" t="s">
-        <v>580</v>
+        <v>2715</v>
       </c>
       <c r="K3899">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3900" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3900" t="s">
-        <v>1244</v>
+        <v>1265</v>
       </c>
       <c r="E3900" t="s">
-        <v>1083</v>
+        <v>1266</v>
       </c>
       <c r="K3900">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3901" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3901" t="s">
-        <v>1221</v>
+        <v>1267</v>
       </c>
       <c r="E3901" t="s">
-        <v>356</v>
+        <v>1266</v>
       </c>
       <c r="K3901">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3902" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3902" t="s">
-        <v>1257</v>
+        <v>1227</v>
       </c>
       <c r="E3902" t="s">
-        <v>620</v>
+        <v>497</v>
       </c>
       <c r="K3902">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3903" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3903" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="E3903" t="s">
         <v>497</v>
       </c>
       <c r="K3903">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3904" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3904" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="E3904" t="s">
         <v>1262</v>
       </c>
       <c r="K3904">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3905" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3905" t="s">
-        <v>3101</v>
+        <v>1252</v>
       </c>
       <c r="E3905" t="s">
-        <v>1262</v>
+        <v>580</v>
       </c>
       <c r="K3905">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3906" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3906" t="s">
-        <v>3102</v>
+        <v>1244</v>
       </c>
       <c r="E3906" t="s">
-        <v>3103</v>
+        <v>1083</v>
       </c>
       <c r="K3906">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3907" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3907" t="s">
-        <v>3503</v>
+        <v>1221</v>
       </c>
       <c r="E3907" t="s">
-        <v>497</v>
+        <v>356</v>
       </c>
       <c r="K3907">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3908" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3908" t="s">
-        <v>3509</v>
+        <v>1257</v>
       </c>
       <c r="E3908" t="s">
         <v>620</v>
       </c>
       <c r="K3908">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3909" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3909" t="s">
-        <v>4872</v>
+        <v>1229</v>
       </c>
       <c r="E3909" t="s">
-        <v>1083</v>
+        <v>497</v>
       </c>
       <c r="K3909">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3910" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3910" t="s">
-        <v>4267</v>
+        <v>1263</v>
       </c>
       <c r="E3910" t="s">
-        <v>741</v>
+        <v>1262</v>
       </c>
       <c r="K3910">
         <v>3.5</v>
@@ -58119,87 +58140,87 @@
     </row>
     <row r="3911" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3911" t="s">
-        <v>4268</v>
+        <v>3101</v>
       </c>
       <c r="E3911" t="s">
-        <v>667</v>
+        <v>1262</v>
       </c>
       <c r="K3911">
-        <v>38</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3912" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3912" t="s">
-        <v>1253</v>
+        <v>3102</v>
       </c>
       <c r="E3912" t="s">
-        <v>667</v>
+        <v>3103</v>
       </c>
       <c r="K3912">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3913" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3913" t="s">
-        <v>678</v>
+        <v>3503</v>
       </c>
       <c r="E3913" t="s">
-        <v>352</v>
+        <v>497</v>
       </c>
       <c r="K3913">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3914" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3914" t="s">
-        <v>3236</v>
+        <v>3509</v>
       </c>
       <c r="E3914" t="s">
-        <v>775</v>
+        <v>620</v>
       </c>
       <c r="K3914">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3915" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3915" t="s">
-        <v>3237</v>
+        <v>4872</v>
       </c>
       <c r="E3915" t="s">
-        <v>775</v>
+        <v>1083</v>
       </c>
       <c r="K3915">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3916" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3916" t="s">
-        <v>3238</v>
+        <v>4267</v>
       </c>
       <c r="E3916" t="s">
-        <v>474</v>
+        <v>741</v>
       </c>
       <c r="K3916">
-        <v>25</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3917" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3917" t="s">
-        <v>3239</v>
+        <v>4268</v>
       </c>
       <c r="E3917" t="s">
         <v>667</v>
       </c>
       <c r="K3917">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3918" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3918" t="s">
-        <v>3240</v>
+        <v>1253</v>
       </c>
       <c r="E3918" t="s">
-        <v>326</v>
+        <v>667</v>
       </c>
       <c r="K3918">
         <v>25</v>
@@ -58207,397 +58228,463 @@
     </row>
     <row r="3919" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3919" t="s">
-        <v>3241</v>
+        <v>678</v>
       </c>
       <c r="E3919" t="s">
         <v>352</v>
       </c>
       <c r="K3919">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3920" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3920" t="s">
-        <v>3242</v>
+        <v>3236</v>
       </c>
       <c r="E3920" t="s">
-        <v>3243</v>
+        <v>775</v>
       </c>
       <c r="K3920">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3921" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3921" t="s">
-        <v>3244</v>
+        <v>3237</v>
       </c>
       <c r="E3921" t="s">
-        <v>287</v>
+        <v>775</v>
       </c>
       <c r="K3921">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3922" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3922" t="s">
-        <v>3921</v>
+        <v>3238</v>
       </c>
       <c r="E3922" t="s">
-        <v>667</v>
+        <v>474</v>
       </c>
       <c r="K3922">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3923" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3923" t="s">
-        <v>3922</v>
+        <v>3239</v>
       </c>
       <c r="E3923" t="s">
-        <v>3923</v>
+        <v>667</v>
       </c>
       <c r="K3923">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3924" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3924" t="s">
-        <v>3924</v>
+        <v>3240</v>
       </c>
       <c r="E3924" t="s">
-        <v>3925</v>
+        <v>326</v>
       </c>
       <c r="K3924">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3925" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3925" t="s">
-        <v>3926</v>
+        <v>3241</v>
       </c>
       <c r="E3925" t="s">
-        <v>791</v>
+        <v>352</v>
       </c>
       <c r="K3925">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3926" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3926" t="s">
-        <v>3927</v>
+        <v>3242</v>
       </c>
       <c r="E3926" t="s">
-        <v>1272</v>
+        <v>3243</v>
       </c>
       <c r="K3926">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3927" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3927" t="s">
-        <v>3928</v>
+        <v>3244</v>
       </c>
       <c r="E3927" t="s">
-        <v>3929</v>
+        <v>287</v>
       </c>
       <c r="K3927">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3928" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3928" t="s">
-        <v>3930</v>
+        <v>3921</v>
       </c>
       <c r="E3928" t="s">
-        <v>3931</v>
+        <v>667</v>
       </c>
       <c r="K3928">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3929" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3929" t="s">
-        <v>3932</v>
+        <v>3922</v>
       </c>
       <c r="E3929" t="s">
-        <v>3933</v>
+        <v>3923</v>
       </c>
       <c r="K3929">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3930" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3930" t="s">
-        <v>3934</v>
+        <v>3924</v>
       </c>
       <c r="E3930" t="s">
-        <v>3935</v>
+        <v>3925</v>
       </c>
       <c r="K3930">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3931" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3931" t="s">
-        <v>3967</v>
+        <v>3926</v>
       </c>
       <c r="E3931" t="s">
-        <v>3968</v>
+        <v>791</v>
       </c>
       <c r="K3931">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3932" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3932" t="s">
-        <v>3969</v>
+        <v>3927</v>
       </c>
       <c r="E3932" t="s">
-        <v>639</v>
+        <v>1272</v>
       </c>
       <c r="K3932">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3933" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3933" t="s">
-        <v>4281</v>
+        <v>3928</v>
       </c>
       <c r="E3933" t="s">
-        <v>667</v>
+        <v>3929</v>
       </c>
       <c r="K3933">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3934" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3934" t="s">
-        <v>4391</v>
+        <v>3930</v>
       </c>
       <c r="E3934" t="s">
-        <v>791</v>
+        <v>3931</v>
       </c>
       <c r="K3934">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3935" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3935" t="s">
-        <v>4654</v>
+        <v>3932</v>
       </c>
       <c r="E3935" t="s">
-        <v>3590</v>
+        <v>3933</v>
       </c>
       <c r="K3935">
-        <v>18</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3936" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3936" t="s">
-        <v>4659</v>
+        <v>3934</v>
       </c>
       <c r="E3936" t="s">
-        <v>4660</v>
+        <v>3935</v>
       </c>
       <c r="K3936">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3937" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3937" t="s">
-        <v>4690</v>
+        <v>3967</v>
       </c>
       <c r="E3937" t="s">
-        <v>153</v>
+        <v>3968</v>
       </c>
       <c r="K3937">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3938" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3938" t="s">
-        <v>4734</v>
+        <v>3969</v>
       </c>
       <c r="E3938" t="s">
-        <v>2507</v>
+        <v>639</v>
       </c>
       <c r="K3938">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3939" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3939" t="s">
-        <v>4735</v>
+        <v>4281</v>
       </c>
       <c r="E3939" t="s">
-        <v>4736</v>
+        <v>667</v>
       </c>
       <c r="K3939">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3940" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3940" t="s">
-        <v>4737</v>
+        <v>4391</v>
       </c>
       <c r="E3940" t="s">
-        <v>3088</v>
+        <v>791</v>
       </c>
       <c r="K3940">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3941" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3941" t="s">
-        <v>4738</v>
+        <v>4654</v>
       </c>
       <c r="E3941" t="s">
-        <v>626</v>
+        <v>3590</v>
       </c>
       <c r="K3941">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3942" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3942" t="s">
-        <v>4739</v>
+        <v>4659</v>
       </c>
       <c r="E3942" t="s">
-        <v>1570</v>
+        <v>4660</v>
       </c>
       <c r="K3942">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3943" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3943" t="s">
-        <v>4740</v>
+        <v>4690</v>
       </c>
       <c r="E3943" t="s">
-        <v>3946</v>
+        <v>153</v>
       </c>
       <c r="K3943">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3944" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3944" t="s">
-        <v>4741</v>
+        <v>4734</v>
       </c>
       <c r="E3944" t="s">
-        <v>626</v>
+        <v>2507</v>
       </c>
       <c r="K3944">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3945" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3945" t="s">
-        <v>4742</v>
+        <v>4735</v>
       </c>
       <c r="E3945" t="s">
-        <v>4743</v>
+        <v>4736</v>
       </c>
       <c r="K3945">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3946" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3946" t="s">
-        <v>4744</v>
+        <v>4737</v>
       </c>
       <c r="E3946" t="s">
-        <v>3946</v>
+        <v>3088</v>
       </c>
       <c r="K3946">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3947" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3947" t="s">
-        <v>4745</v>
+        <v>4738</v>
       </c>
       <c r="E3947" t="s">
-        <v>3946</v>
+        <v>626</v>
       </c>
       <c r="K3947">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3948" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3948" t="s">
-        <v>4753</v>
+        <v>4739</v>
       </c>
       <c r="E3948" t="s">
         <v>1570</v>
       </c>
       <c r="K3948">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3949" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3949" t="s">
-        <v>4760</v>
+        <v>4740</v>
       </c>
       <c r="E3949" t="s">
-        <v>756</v>
+        <v>3946</v>
       </c>
       <c r="K3949">
-        <v>3.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3950" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3950" t="s">
-        <v>4761</v>
+        <v>4741</v>
       </c>
       <c r="E3950" t="s">
-        <v>756</v>
+        <v>626</v>
       </c>
       <c r="K3950">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3951" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3951" t="s">
-        <v>4762</v>
+        <v>4742</v>
       </c>
       <c r="E3951" t="s">
-        <v>3946</v>
+        <v>4743</v>
       </c>
       <c r="K3951">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3952" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3952" t="s">
-        <v>4811</v>
+        <v>4744</v>
       </c>
       <c r="E3952" t="s">
         <v>3946</v>
       </c>
       <c r="K3952">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3953" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3953" t="s">
-        <v>4815</v>
+        <v>4745</v>
       </c>
       <c r="E3953" t="s">
         <v>3946</v>
       </c>
       <c r="K3953">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3954" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3954" t="s">
+        <v>4753</v>
+      </c>
+      <c r="E3954" t="s">
+        <v>1570</v>
+      </c>
+      <c r="K3954">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3955" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3955" t="s">
+        <v>4760</v>
+      </c>
+      <c r="E3955" t="s">
+        <v>756</v>
+      </c>
+      <c r="K3955">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3956" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3956" t="s">
+        <v>4761</v>
+      </c>
+      <c r="E3956" t="s">
+        <v>756</v>
+      </c>
+      <c r="K3956">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3957" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3957" t="s">
+        <v>4762</v>
+      </c>
+      <c r="E3957" t="s">
+        <v>3946</v>
+      </c>
+      <c r="K3957">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3958" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3958" t="s">
+        <v>4811</v>
+      </c>
+      <c r="E3958" t="s">
+        <v>3946</v>
+      </c>
+      <c r="K3958">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3959" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3959" t="s">
+        <v>4815</v>
+      </c>
+      <c r="E3959" t="s">
+        <v>3946</v>
+      </c>
+      <c r="K3959">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3960" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3960" t="s">
         <v>4818</v>
       </c>
-      <c r="E3954" t="s">
+      <c r="E3960" t="s">
         <v>3946</v>
       </c>
-      <c r="K3954">
+      <c r="K3960">
         <v>12</v>
       </c>
     </row>

</xml_diff>